<commit_message>
compare policy of different facility of health system
</commit_message>
<xml_diff>
--- a/Features/Audit.xlsx
+++ b/Features/Audit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB0F9F4-9D6B-43F9-B0D2-F6DC2FE50EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6922B469-996C-420D-A6F5-236B09DF1124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9036" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2132,6 +2132,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2144,12 +2219,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2158,75 +2227,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2807,16 +2807,16 @@
       <c r="A2" s="83">
         <v>4</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="73" t="s">
         <v>35</v>
       </c>
       <c r="D2" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="82">
+      <c r="E2" s="71">
         <v>5</v>
       </c>
       <c r="F2" s="50" t="s">
@@ -2828,7 +2828,7 @@
       <c r="H2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="69">
+      <c r="I2" s="94">
         <v>6</v>
       </c>
       <c r="J2" s="47" t="s">
@@ -2840,10 +2840,10 @@
       <c r="L2" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="72">
+      <c r="M2" s="95">
         <v>11</v>
       </c>
-      <c r="N2" s="66" t="s">
+      <c r="N2" s="91" t="s">
         <v>96</v>
       </c>
       <c r="O2" s="32" t="s">
@@ -2855,10 +2855,10 @@
     </row>
     <row r="3" spans="1:16" ht="93.75" customHeight="1">
       <c r="A3" s="84"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="92"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="84"/>
-      <c r="E3" s="76"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="51"/>
       <c r="G3" s="30" t="s">
         <v>36</v>
@@ -2866,7 +2866,7 @@
       <c r="H3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="70"/>
+      <c r="I3" s="78"/>
       <c r="J3" s="48"/>
       <c r="K3" s="31" t="s">
         <v>36</v>
@@ -2874,8 +2874,8 @@
       <c r="L3" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="73"/>
-      <c r="N3" s="67"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="92"/>
       <c r="O3" s="32" t="s">
         <v>36</v>
       </c>
@@ -2885,10 +2885,10 @@
     </row>
     <row r="4" spans="1:16" ht="45" customHeight="1">
       <c r="A4" s="84"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="76"/>
       <c r="D4" s="84"/>
-      <c r="E4" s="76"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="51"/>
       <c r="G4" s="30" t="s">
         <v>37</v>
@@ -2896,7 +2896,7 @@
       <c r="H4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="70"/>
+      <c r="I4" s="78"/>
       <c r="J4" s="48"/>
       <c r="K4" s="31" t="s">
         <v>37</v>
@@ -2904,17 +2904,17 @@
       <c r="L4" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="68"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="93"/>
       <c r="O4" s="13"/>
       <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:16" ht="31.5" customHeight="1">
       <c r="A5" s="84"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="92"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="76"/>
       <c r="D5" s="84"/>
-      <c r="E5" s="76"/>
+      <c r="E5" s="87"/>
       <c r="F5" s="51"/>
       <c r="G5" s="30" t="s">
         <v>62</v>
@@ -2922,7 +2922,7 @@
       <c r="H5" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="70"/>
+      <c r="I5" s="78"/>
       <c r="J5" s="48"/>
       <c r="K5" s="12"/>
       <c r="L5" s="15"/>
@@ -2933,10 +2933,10 @@
     </row>
     <row r="6" spans="1:16" ht="31.5" customHeight="1">
       <c r="A6" s="84"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="92"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="84"/>
-      <c r="E6" s="76"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="51"/>
       <c r="G6" s="30" t="s">
         <v>63</v>
@@ -2944,7 +2944,7 @@
       <c r="H6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="70"/>
+      <c r="I6" s="78"/>
       <c r="J6" s="48"/>
       <c r="K6" s="12"/>
       <c r="L6" s="15"/>
@@ -2955,10 +2955,10 @@
     </row>
     <row r="7" spans="1:16" ht="31.5" customHeight="1">
       <c r="A7" s="84"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="93"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="84"/>
-      <c r="E7" s="77"/>
+      <c r="E7" s="72"/>
       <c r="F7" s="52"/>
       <c r="G7" s="30" t="s">
         <v>64</v>
@@ -2966,7 +2966,7 @@
       <c r="H7" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="71"/>
+      <c r="I7" s="79"/>
       <c r="J7" s="49"/>
       <c r="K7" s="12"/>
       <c r="L7" s="15"/>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="8" spans="1:16" ht="51" customHeight="1">
       <c r="A8" s="84"/>
-      <c r="B8" s="76"/>
+      <c r="B8" s="87"/>
       <c r="C8" s="35" t="s">
         <v>36</v>
       </c>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="9" spans="1:16" ht="31.5" customHeight="1" thickBot="1">
       <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="28" t="s">
         <v>37</v>
       </c>
@@ -3029,19 +3029,19 @@
       <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:16" ht="83.25" customHeight="1">
-      <c r="A11" s="94">
+      <c r="A11" s="67">
         <v>7</v>
       </c>
       <c r="B11" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="75" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="86">
         <v>8</v>
       </c>
       <c r="F11" s="57" t="s">
@@ -3053,10 +3053,10 @@
       <c r="H11" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="81">
+      <c r="I11" s="77">
         <v>6</v>
       </c>
-      <c r="J11" s="78" t="s">
+      <c r="J11" s="80" t="s">
         <v>50</v>
       </c>
       <c r="K11" s="39" t="s">
@@ -3065,10 +3065,10 @@
       <c r="L11" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="81">
+      <c r="M11" s="77">
         <v>11</v>
       </c>
-      <c r="N11" s="78" t="s">
+      <c r="N11" s="80" t="s">
         <v>96</v>
       </c>
       <c r="O11" s="40" t="s">
@@ -3079,11 +3079,11 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="61.5" customHeight="1">
-      <c r="A12" s="95"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="54"/>
-      <c r="C12" s="92"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="45"/>
-      <c r="E12" s="76"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="58"/>
       <c r="G12" s="30" t="s">
         <v>36</v>
@@ -3091,16 +3091,16 @@
       <c r="H12" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="70"/>
-      <c r="J12" s="79"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="81"/>
       <c r="K12" s="31" t="s">
         <v>36</v>
       </c>
       <c r="L12" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="M12" s="70"/>
-      <c r="N12" s="79"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="81"/>
       <c r="O12" s="34" t="s">
         <v>36</v>
       </c>
@@ -3109,11 +3109,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="30.75" customHeight="1">
-      <c r="A13" s="95"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="54"/>
-      <c r="C13" s="93"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="46"/>
-      <c r="E13" s="77"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="59"/>
       <c r="G13" s="30" t="s">
         <v>37</v>
@@ -3121,29 +3121,29 @@
       <c r="H13" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="71"/>
-      <c r="J13" s="80"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="82"/>
       <c r="K13" s="31" t="s">
         <v>37</v>
       </c>
       <c r="L13" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="M13" s="71"/>
-      <c r="N13" s="80"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="82"/>
       <c r="O13" s="15"/>
       <c r="P13" s="14"/>
     </row>
     <row r="14" spans="1:16" ht="43.2">
-      <c r="A14" s="95"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="54"/>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="73" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="82">
+      <c r="E14" s="71">
         <v>11</v>
       </c>
       <c r="F14" s="89" t="s">
@@ -3165,12 +3165,12 @@
       <c r="P14" s="14"/>
     </row>
     <row r="15" spans="1:16" ht="72">
-      <c r="A15" s="95"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="54"/>
-      <c r="C15" s="93"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="46"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="80"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="82"/>
       <c r="G15" s="30" t="s">
         <v>36</v>
       </c>
@@ -3187,7 +3187,7 @@
       <c r="P15" s="14"/>
     </row>
     <row r="16" spans="1:16" ht="28.8">
-      <c r="A16" s="95"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="54"/>
       <c r="C16" s="35" t="s">
         <v>37</v>
@@ -3209,7 +3209,7 @@
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" ht="60" customHeight="1" thickBot="1">
-      <c r="A17" s="96"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="55"/>
       <c r="C17" s="36" t="s">
         <v>62</v>
@@ -3231,19 +3231,19 @@
       <c r="P17" s="25"/>
     </row>
     <row r="19" spans="1:16" ht="60" customHeight="1">
-      <c r="A19" s="88">
+      <c r="A19" s="70">
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="88" t="s">
+      <c r="C19" s="70" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="88">
+      <c r="E19" s="70">
         <v>10</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -3255,10 +3255,10 @@
       <c r="H19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I19" s="88">
+      <c r="I19" s="70">
         <v>6</v>
       </c>
-      <c r="J19" s="87" t="s">
+      <c r="J19" s="66" t="s">
         <v>78</v>
       </c>
       <c r="K19" t="s">
@@ -3267,10 +3267,10 @@
       <c r="L19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M19" s="88">
+      <c r="M19" s="70">
         <v>11</v>
       </c>
-      <c r="N19" s="87" t="s">
+      <c r="N19" s="66" t="s">
         <v>96</v>
       </c>
       <c r="O19" t="s">
@@ -3281,11 +3281,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="60" customHeight="1">
-      <c r="A20" s="88"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="88"/>
+      <c r="C20" s="70"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="88"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
         <v>36</v>
@@ -3293,16 +3293,16 @@
       <c r="H20" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="88"/>
-      <c r="J20" s="87"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="66"/>
       <c r="K20" t="s">
         <v>36</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M20" s="88"/>
-      <c r="N20" s="87"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="66"/>
       <c r="O20" t="s">
         <v>36</v>
       </c>
@@ -3311,7 +3311,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="60" customHeight="1">
-      <c r="A21" s="88"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
         <v>36</v>
@@ -3319,19 +3319,19 @@
       <c r="D21" t="s">
         <v>76</v>
       </c>
-      <c r="I21" s="88"/>
-      <c r="J21" s="87"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="66"/>
       <c r="K21" t="s">
         <v>37</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M21" s="88"/>
-      <c r="N21" s="87"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="66"/>
     </row>
     <row r="22" spans="1:16" ht="60" customHeight="1">
-      <c r="A22" s="88"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>37</v>
@@ -3341,7 +3341,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="60" customHeight="1">
-      <c r="A23" s="88"/>
+      <c r="A23" s="70"/>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
         <v>62</v>
@@ -3353,6 +3353,21 @@
     <row r="26" spans="1:16" ht="19.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="M19:M21"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="C2:C7"/>
     <mergeCell ref="N19:N21"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A23"/>
@@ -3363,21 +3378,6 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="M19:M21"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="N11:N13"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="E2:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3388,8 +3388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A478CD3-0361-4E94-991E-870B75BF8680}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3809,7 +3809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F1025B-47DE-4082-9560-1756E510CF14}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>